<commit_message>
Added project planning images
</commit_message>
<xml_diff>
--- a/Project_Planning/Evidence of KSBs.xlsx
+++ b/Project_Planning/Evidence of KSBs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reece\OneDrive\Documents\QAA\EPA\Project_Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F553F731-CF20-4CAF-A28B-FB74B5D6B30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164D0F5C-64C8-42F8-A196-CE2678F2FF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{505748FB-3EEB-4608-916B-AD7B456A714F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="74">
   <si>
     <t>KSB</t>
   </si>
@@ -74,9 +74,6 @@
     <t>S17: Code in a general-purpose programming language.</t>
   </si>
   <si>
-    <t>S20: Writing code in such a way that makes merging easier and facilitates branching by abstraction - i.e., feature toggling</t>
-  </si>
-  <si>
     <t>K5: A range of modern security tools and techniques - e.g. threat modelling, vulnerability scanning and dependency checking, with a general awareness of penetration testing - in order to deal with threats and attack vectors within code and across the cyber domain.</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
   </si>
   <si>
     <t>S22: Incremental refactoring by applying small behaviour-preserving code changes to evolve the architecture.</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Evidence of labels and alt tags used for images and forms within the Frontend HTML and JS files</t>
@@ -265,6 +259,21 @@
     <t xml:space="preserve">https://github.com/Reece-elder/EPA-Sample_Project/blob/main/Project_Planning/images/Simple_front_back.drawio.png
 https://github.com/Reece-elder/EPA-Sample_Project/tree/Dev/DevOps/k8s
 </t>
+  </si>
+  <si>
+    <t>Vulnerabilities have been addressed and covered by writing a risk assessment looking at the possibilities of what could go wrong and how to mitigate the risks through careful consideration and planning</t>
+  </si>
+  <si>
+    <t>S20: Writing code in such a way that makes merging easier and facilitates branching by abstraction</t>
+  </si>
+  <si>
+    <t>Writing simpler code with smaller commits affecting less files makes commits simpler with less merge conflicts to deal with.</t>
+  </si>
+  <si>
+    <t>User Stories have been implemented in the GitHub Projects tab showing a personification of the technical requirements. The user stories have been populated with technical tasks and definitions of done.</t>
+  </si>
+  <si>
+    <t>https://github.com/Reece-elder/EPA-Sample_Project/projects?query=is%3Aopen</t>
   </si>
 </sst>
 </file>
@@ -334,8 +343,8 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -669,296 +678,317 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D5CF9C-B862-44AD-8697-732D8E94EC36}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="83.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="77.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="104.85546875" customWidth="1"/>
+    <col min="1" max="1" width="83.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="77.88671875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="104.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="B26" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    </row>
+    <row r="31" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>16</v>
+      <c r="B31" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -978,8 +1008,9 @@
     <hyperlink ref="C12" r:id="rId8" xr:uid="{EE85B5C7-6D53-4835-90AD-F4AE8254EC8C}"/>
     <hyperlink ref="C28" r:id="rId9" display="https://github.com/Reece-elder/EPA-Sample_Project/blob/main/Project_Planning/images/Simple_front_back.drawio.png_x000a_" xr:uid="{FF15C834-C746-4563-852F-469EC60CB1C5}"/>
     <hyperlink ref="C23" r:id="rId10" xr:uid="{D8E4CE48-9354-4247-B9EF-C44BD5EE3A2A}"/>
+    <hyperlink ref="C18" r:id="rId11" xr:uid="{20FB4AF9-3D7B-4516-B897-FEF17C138F9E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>